<commit_message>
Updated the visualization to show colors as per cell-interactions for an Anatomical Structure 08262021
</commit_message>
<xml_diff>
--- a/Testing_Data_structures_for_cytoscape/Combined_Azimuth_datasets.xlsx
+++ b/Testing_Data_structures_for_cytoscape/Combined_Azimuth_datasets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b73f372793c4b5ce/Desktop/Vikrant/IUB_MS_DS_Coursework/Part_Time_applications/CyberNetworkInfrastructure_RA_Position/Testing_Data_structures_for_cytoscape/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b73f372793c4b5ce/Desktop/Vikrant/Azimuth_Dataset_CNS_Test/Testing_Data_structures_for_cytoscape/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="123" documentId="11_F25DC773A252ABDACC10482BC95A7D325ADE58F2" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F53FD41E-8077-4938-8EA1-03C35A9FBD72}"/>
@@ -11599,7 +11599,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>